<commit_message>
Add collect data at session grid
</commit_message>
<xml_diff>
--- a/Database structure.xlsx
+++ b/Database structure.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Exchanger\Volume_F\Netology\Homework\Graduate work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programm.File\OpenServer\domains\WebDevDiplomaV1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4744A995-8DB8-4142-BC26-C667CB09AFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B895B11F-724D-4041-81BB-A96CA8EAF478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
   <si>
     <t>Структура базы данных</t>
   </si>
@@ -281,57 +281,12 @@
     <t>Фильм5</t>
   </si>
   <si>
-    <t>Фильм6</t>
-  </si>
-  <si>
     <t>Красный1</t>
   </si>
   <si>
-    <t>Фильм7</t>
-  </si>
-  <si>
-    <t>Фильм8</t>
-  </si>
-  <si>
-    <t>Фильм9</t>
-  </si>
-  <si>
-    <t>Фильм10</t>
-  </si>
-  <si>
-    <t>Фильм11</t>
-  </si>
-  <si>
-    <t>Фильм12</t>
-  </si>
-  <si>
-    <t>Фильм13</t>
-  </si>
-  <si>
     <t>Зеленый1</t>
   </si>
   <si>
-    <t>Фильм14</t>
-  </si>
-  <si>
-    <t>Фильм15</t>
-  </si>
-  <si>
-    <t>Фильм16</t>
-  </si>
-  <si>
-    <t>Фильм17</t>
-  </si>
-  <si>
-    <t>Фильм18</t>
-  </si>
-  <si>
-    <t>Фильм19</t>
-  </si>
-  <si>
-    <t>Фильм20</t>
-  </si>
-  <si>
     <t>См. примечание</t>
   </si>
   <si>
@@ -357,6 +312,24 @@
   </si>
   <si>
     <t>В таблицу users добавить столбец status - для разграничения прав доступа</t>
+  </si>
+  <si>
+    <t>Таблица session_grid old</t>
+  </si>
+  <si>
+    <t>sesStart</t>
+  </si>
+  <si>
+    <t>admission</t>
+  </si>
+  <si>
+    <t>idHall</t>
+  </si>
+  <si>
+    <t>idFilm</t>
+  </si>
+  <si>
+    <t>2023-08-06</t>
   </si>
 </sst>
 </file>
@@ -416,7 +389,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -514,26 +487,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -562,9 +520,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -578,6 +533,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -858,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,44 +836,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
+      <c r="A2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -936,16 +895,16 @@
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>52</v>
+      <c r="I4" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -973,11 +932,11 @@
       <c r="H5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>53</v>
+      <c r="I5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1005,17 +964,17 @@
       <c r="J7" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1050,7 +1009,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E11" s="4">
         <v>300</v>
@@ -1068,10 +1027,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E12" s="5">
         <v>250</v>
@@ -1089,7 +1048,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6">
@@ -1101,15 +1060,15 @@
       <c r="H13" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
+      <c r="A15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1126,7 +1085,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>21</v>
@@ -1152,7 +1111,7 @@
         <v>45079</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F17" s="10">
         <v>0.41666666666666669</v>
@@ -1161,7 +1120,7 @@
         <v>13</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1178,7 +1137,7 @@
         <v>45079</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F18" s="13">
         <v>0.5</v>
@@ -1187,7 +1146,7 @@
         <v>25</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1204,7 +1163,7 @@
         <v>45079</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F19" s="13">
         <v>0.58333333333333337</v>
@@ -1213,7 +1172,7 @@
         <v>26</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1230,7 +1189,7 @@
         <v>45079</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F20" s="13">
         <v>0.66666666666666663</v>
@@ -1239,7 +1198,7 @@
         <v>27</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1256,7 +1215,7 @@
         <v>45079</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F21" s="13">
         <v>0.75</v>
@@ -1265,7 +1224,7 @@
         <v>28</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1282,7 +1241,7 @@
         <v>45079</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F22" s="13">
         <v>0.83333333333333304</v>
@@ -1291,406 +1250,56 @@
         <v>29</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
-        <v>7</v>
-      </c>
-      <c r="B23" s="11">
-        <v>7</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="13">
-        <v>0.91666666666666596</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
-        <v>8</v>
-      </c>
-      <c r="B24" s="11">
-        <v>8</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="13">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="G24" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
-        <v>9</v>
-      </c>
-      <c r="B25" s="11">
-        <v>9</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>47</v>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
-        <v>10</v>
-      </c>
-      <c r="B26" s="11">
-        <v>10</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="13">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
-        <v>11</v>
-      </c>
-      <c r="B27" s="11">
-        <v>11</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="13">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
-        <v>12</v>
-      </c>
-      <c r="B28" s="11">
-        <v>12</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="13">
-        <v>0.75</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="11">
-        <v>13</v>
-      </c>
-      <c r="B29" s="11">
-        <v>13</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="13">
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
-        <v>14</v>
-      </c>
-      <c r="B30" s="11">
-        <v>14</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="13">
-        <v>0.91666666666666596</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
-        <v>15</v>
-      </c>
-      <c r="B31" s="11">
-        <v>15</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F31" s="13">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H31" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="11">
-        <v>16</v>
-      </c>
-      <c r="B32" s="11">
-        <v>16</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F32" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="11">
-        <v>17</v>
-      </c>
-      <c r="B33" s="11">
-        <v>17</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F33" s="13">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
-        <v>18</v>
-      </c>
-      <c r="B34" s="11">
-        <v>18</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34" s="13">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="11">
-        <v>19</v>
-      </c>
-      <c r="B35" s="11">
-        <v>19</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="13">
-        <v>0.75</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="11">
-        <v>20</v>
-      </c>
-      <c r="B36" s="11">
-        <v>20</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="12">
-        <v>45079</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F36" s="13">
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="14">
-        <v>21</v>
-      </c>
-      <c r="B37" s="14">
-        <v>21</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="15">
-        <v>45079</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" s="16">
-        <v>0.91666666666666596</v>
-      </c>
-      <c r="G37" s="14" t="s">
+      <c r="C26" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H37" s="14" t="s">
-        <v>47</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A9:I9"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="A2:J2"/>
+    <mergeCell ref="B24:H24"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>